<commit_message>
user verifcation crashes in date util
</commit_message>
<xml_diff>
--- a/merlinserver/src/main/resources/data.xlsx
+++ b/merlinserver/src/main/resources/data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luie\Desktop\work\revature\project2\Server\Merlin\merlinserver\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Alex\MerlinServerGitBash\Merlin\merlinserver\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19845" windowHeight="9105" xr2:uid="{D43942BD-B1C4-444E-A31D-5DDE6591484D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19845" windowHeight="9105"/>
   </bookViews>
   <sheets>
     <sheet name="dateformats" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>dd-MM-yyyy</t>
   </si>
@@ -117,19 +117,27 @@
   </si>
   <si>
     <t>MMMM dd, yyyy hh:mm:ss a</t>
+  </si>
+  <si>
+    <t>ddd MMM dd HH:mm:ss yyyy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7D2727"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,8 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,174 +478,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD381E2-994D-402D-8D15-FD36FC430DCE}">
-  <dimension ref="A1:A31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>